<commit_message>
Got dem beetr pictures doe
</commit_message>
<xml_diff>
--- a/classification.xlsx
+++ b/classification.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="2">
   <si>
     <t>positive</t>
   </si>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W75"/>
+  <dimension ref="A1:W77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W75"/>
+      <selection sqref="A1:W77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5691,6 +5691,148 @@
       </c>
       <c r="W75">
         <v>0.15790382271295919</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>4902.965208700517</v>
+      </c>
+      <c r="C76">
+        <v>909.77832594394704</v>
+      </c>
+      <c r="D76">
+        <v>-196.35657995417239</v>
+      </c>
+      <c r="E76">
+        <v>-260.95010508196384</v>
+      </c>
+      <c r="F76">
+        <v>-361.32977743852831</v>
+      </c>
+      <c r="G76">
+        <v>3501.8361177763713</v>
+      </c>
+      <c r="H76">
+        <v>-402.82888923917517</v>
+      </c>
+      <c r="I76">
+        <v>-131.85398300954628</v>
+      </c>
+      <c r="J76">
+        <v>-30.399506203604364</v>
+      </c>
+      <c r="K76">
+        <v>-55.317171646238855</v>
+      </c>
+      <c r="L76">
+        <v>-340.32066931272715</v>
+      </c>
+      <c r="M76">
+        <v>-92.37166566066287</v>
+      </c>
+      <c r="N76">
+        <v>-24.32915355370805</v>
+      </c>
+      <c r="O76">
+        <v>-62.111510173449886</v>
+      </c>
+      <c r="P76">
+        <v>668.56844620231789</v>
+      </c>
+      <c r="Q76">
+        <v>-94.521377930635964</v>
+      </c>
+      <c r="R76">
+        <v>18.32991108093951</v>
+      </c>
+      <c r="S76">
+        <v>84.367770846312268</v>
+      </c>
+      <c r="T76">
+        <v>315.61835965303032</v>
+      </c>
+      <c r="U76">
+        <v>-61.323159791283821</v>
+      </c>
+      <c r="V76">
+        <v>-12.852829714954414</v>
+      </c>
+      <c r="W76">
+        <v>-1.2848959438638907</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>1.4757616550993236</v>
+      </c>
+      <c r="C77">
+        <v>2.1772607417544743</v>
+      </c>
+      <c r="D77">
+        <v>3.0434831170432886</v>
+      </c>
+      <c r="E77">
+        <v>1.2415832626413441</v>
+      </c>
+      <c r="F77">
+        <v>1.2457268877900551</v>
+      </c>
+      <c r="G77">
+        <v>0.56126587903722047</v>
+      </c>
+      <c r="H77">
+        <v>1.1743272631947785</v>
+      </c>
+      <c r="I77">
+        <v>0.23054550741241203</v>
+      </c>
+      <c r="J77">
+        <v>-3.4261782347163527</v>
+      </c>
+      <c r="K77">
+        <v>0.66334587487468022</v>
+      </c>
+      <c r="L77">
+        <v>1.0306370471546036</v>
+      </c>
+      <c r="M77">
+        <v>0.76256777522881058</v>
+      </c>
+      <c r="N77">
+        <v>1.2988415213542728</v>
+      </c>
+      <c r="O77">
+        <v>2.4136597060060243</v>
+      </c>
+      <c r="P77">
+        <v>1.2247158941234109</v>
+      </c>
+      <c r="Q77">
+        <v>131.36807363693123</v>
+      </c>
+      <c r="R77">
+        <v>0.50972075458921062</v>
+      </c>
+      <c r="S77">
+        <v>1.623167155359619</v>
+      </c>
+      <c r="T77">
+        <v>2.1677719788989656</v>
+      </c>
+      <c r="U77">
+        <v>-0.26018393796375672</v>
+      </c>
+      <c r="V77">
+        <v>6.8111669711356573</v>
+      </c>
+      <c r="W77">
+        <v>-2.5626701301248795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>